<commit_message>
trying to get two runs showed in fsx
</commit_message>
<xml_diff>
--- a/runs/MaxQuantAnalysis/isa.run.xlsx
+++ b/runs/MaxQuantAnalysis/isa.run.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="isa_run" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="NewTable0" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>RUN</t>
   </si>
@@ -95,6 +96,24 @@
   </si>
   <si>
     <t>Run Person Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>Input [Source Name]</t>
+  </si>
+  <si>
+    <t>Output [Sample Name]</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bc</t>
   </si>
 </sst>
 </file>
@@ -147,6 +166,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable0" displayName="annotationTable0" ref="A1:B3" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:B3">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Output [Sample Name]" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,4 +620,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>